<commit_message>
Remove unnecessary Excel tabs and update screenshot
</commit_message>
<xml_diff>
--- a/pareto/examples/visualization_demos/plot_bars/plot_bars_demo.xlsx
+++ b/pareto/examples/visualization_demos/plot_bars/plot_bars_demo.xlsx
@@ -5,18 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\examples\visualization_demos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\examples\visualization_demos\plot_bars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4585DBCB-E821-4811-9DA5-B373871C8482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EF0AF6-326E-46B6-BD48-9A8CA49A0F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{46113138-D233-4404-A744-E7E1E9C0AFA2}"/>
   </bookViews>
   <sheets>
     <sheet name="v_F_Trucked_Static" sheetId="3" r:id="rId1"/>
     <sheet name="v_F_Trucked" sheetId="1" r:id="rId2"/>
-    <sheet name="v_L_PadStorage_T" sheetId="5" r:id="rId3"/>
-    <sheet name="v_L_PadStorage_Static" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">v_F_Trucked!$A$2:$D$1322</definedName>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6880" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6607" uniqueCount="400">
   <si>
     <t>Origin</t>
   </si>
@@ -1241,381 +1239,6 @@
   </si>
   <si>
     <t>Mar-17-2022</t>
-  </si>
-  <si>
-    <t>Completion pad</t>
-  </si>
-  <si>
-    <t>Storage Levels</t>
-  </si>
-  <si>
-    <t>T01</t>
-  </si>
-  <si>
-    <t>T02</t>
-  </si>
-  <si>
-    <t>T44</t>
-  </si>
-  <si>
-    <t>T45</t>
-  </si>
-  <si>
-    <t>T46</t>
-  </si>
-  <si>
-    <t>T47</t>
-  </si>
-  <si>
-    <t>T48</t>
-  </si>
-  <si>
-    <t>T49</t>
-  </si>
-  <si>
-    <t>T50</t>
-  </si>
-  <si>
-    <t>T70</t>
-  </si>
-  <si>
-    <t>T03</t>
-  </si>
-  <si>
-    <t>T04</t>
-  </si>
-  <si>
-    <t>T05</t>
-  </si>
-  <si>
-    <t>T06</t>
-  </si>
-  <si>
-    <t>T07</t>
-  </si>
-  <si>
-    <t>T08</t>
-  </si>
-  <si>
-    <t>T09</t>
-  </si>
-  <si>
-    <t>T10</t>
-  </si>
-  <si>
-    <t>T11</t>
-  </si>
-  <si>
-    <t>T12</t>
-  </si>
-  <si>
-    <t>T13</t>
-  </si>
-  <si>
-    <t>T14</t>
-  </si>
-  <si>
-    <t>T15</t>
-  </si>
-  <si>
-    <t>T16</t>
-  </si>
-  <si>
-    <t>T17</t>
-  </si>
-  <si>
-    <t>T18</t>
-  </si>
-  <si>
-    <t>T19</t>
-  </si>
-  <si>
-    <t>T20</t>
-  </si>
-  <si>
-    <t>T21</t>
-  </si>
-  <si>
-    <t>T22</t>
-  </si>
-  <si>
-    <t>T23</t>
-  </si>
-  <si>
-    <t>T24</t>
-  </si>
-  <si>
-    <t>T25</t>
-  </si>
-  <si>
-    <t>T26</t>
-  </si>
-  <si>
-    <t>T27</t>
-  </si>
-  <si>
-    <t>T28</t>
-  </si>
-  <si>
-    <t>T29</t>
-  </si>
-  <si>
-    <t>T30</t>
-  </si>
-  <si>
-    <t>T31</t>
-  </si>
-  <si>
-    <t>T32</t>
-  </si>
-  <si>
-    <t>T33</t>
-  </si>
-  <si>
-    <t>T34</t>
-  </si>
-  <si>
-    <t>T35</t>
-  </si>
-  <si>
-    <t>T36</t>
-  </si>
-  <si>
-    <t>T37</t>
-  </si>
-  <si>
-    <t>T38</t>
-  </si>
-  <si>
-    <t>T39</t>
-  </si>
-  <si>
-    <t>T40</t>
-  </si>
-  <si>
-    <t>T41</t>
-  </si>
-  <si>
-    <t>T42</t>
-  </si>
-  <si>
-    <t>T43</t>
-  </si>
-  <si>
-    <t>T51</t>
-  </si>
-  <si>
-    <t>T52</t>
-  </si>
-  <si>
-    <t>T53</t>
-  </si>
-  <si>
-    <t>T54</t>
-  </si>
-  <si>
-    <t>T55</t>
-  </si>
-  <si>
-    <t>T56</t>
-  </si>
-  <si>
-    <t>T57</t>
-  </si>
-  <si>
-    <t>T58</t>
-  </si>
-  <si>
-    <t>T59</t>
-  </si>
-  <si>
-    <t>T60</t>
-  </si>
-  <si>
-    <t>T61</t>
-  </si>
-  <si>
-    <t>T62</t>
-  </si>
-  <si>
-    <t>T63</t>
-  </si>
-  <si>
-    <t>T64</t>
-  </si>
-  <si>
-    <t>T65</t>
-  </si>
-  <si>
-    <t>T66</t>
-  </si>
-  <si>
-    <t>T67</t>
-  </si>
-  <si>
-    <t>T68</t>
-  </si>
-  <si>
-    <t>T69</t>
-  </si>
-  <si>
-    <t>T71</t>
-  </si>
-  <si>
-    <t>T72</t>
-  </si>
-  <si>
-    <t>T73</t>
-  </si>
-  <si>
-    <t>T74</t>
-  </si>
-  <si>
-    <t>T75</t>
-  </si>
-  <si>
-    <t>T76</t>
-  </si>
-  <si>
-    <t>T77</t>
-  </si>
-  <si>
-    <t>T78</t>
-  </si>
-  <si>
-    <t>T79</t>
-  </si>
-  <si>
-    <t>T80</t>
-  </si>
-  <si>
-    <t>T81</t>
-  </si>
-  <si>
-    <t>T82</t>
-  </si>
-  <si>
-    <t>T83</t>
-  </si>
-  <si>
-    <t>T84</t>
-  </si>
-  <si>
-    <t>T85</t>
-  </si>
-  <si>
-    <t>T86</t>
-  </si>
-  <si>
-    <t>T87</t>
-  </si>
-  <si>
-    <t>T88</t>
-  </si>
-  <si>
-    <t>T89</t>
-  </si>
-  <si>
-    <t>T90</t>
-  </si>
-  <si>
-    <t>T91</t>
-  </si>
-  <si>
-    <t>T92</t>
-  </si>
-  <si>
-    <t>T93</t>
-  </si>
-  <si>
-    <t>T94</t>
-  </si>
-  <si>
-    <t>T95</t>
-  </si>
-  <si>
-    <t>T96</t>
-  </si>
-  <si>
-    <t>T97</t>
-  </si>
-  <si>
-    <t>T98</t>
-  </si>
-  <si>
-    <t>T99</t>
-  </si>
-  <si>
-    <t>T100</t>
-  </si>
-  <si>
-    <t>T101</t>
-  </si>
-  <si>
-    <t>T102</t>
-  </si>
-  <si>
-    <t>T103</t>
-  </si>
-  <si>
-    <t>T104</t>
-  </si>
-  <si>
-    <t>T105</t>
-  </si>
-  <si>
-    <t>T106</t>
-  </si>
-  <si>
-    <t>T107</t>
-  </si>
-  <si>
-    <t>T108</t>
-  </si>
-  <si>
-    <t>T109</t>
-  </si>
-  <si>
-    <t>T110</t>
-  </si>
-  <si>
-    <t>T111</t>
-  </si>
-  <si>
-    <t>T112</t>
-  </si>
-  <si>
-    <t>T113</t>
-  </si>
-  <si>
-    <t>T114</t>
-  </si>
-  <si>
-    <t>T115</t>
-  </si>
-  <si>
-    <t>T116</t>
-  </si>
-  <si>
-    <t>T117</t>
-  </si>
-  <si>
-    <t>T118</t>
-  </si>
-  <si>
-    <t>T119</t>
-  </si>
-  <si>
-    <t>T120</t>
-  </si>
-  <si>
-    <t>T121</t>
-  </si>
-  <si>
-    <t>T122</t>
-  </si>
-  <si>
-    <t>T123</t>
   </si>
 </sst>
 </file>
@@ -1672,12 +1295,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -35059,1542 +34678,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB323BC-97DA-4AA8-8085-B093B5D97FCD}">
-  <dimension ref="A2:C134"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>400</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="C3" s="5">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="C4" s="5">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="C6" s="5">
-        <v>3200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="C7" s="5">
-        <v>5700</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="C8" s="5">
-        <v>7200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="C9" s="5">
-        <v>8600</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="C10" s="5">
-        <v>10300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="C11" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="C13" s="5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="C14" s="5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="C15" s="5">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="C16" s="5">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="C17" s="5">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="C18" s="5">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>418</v>
-      </c>
-      <c r="C19" s="5">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="C20" s="5">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="C21" s="5">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="C22" s="5">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="C23" s="5">
-        <v>3300</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="C24" s="5">
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="C25" s="5">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="C26" s="5">
-        <v>3700</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="C27" s="5">
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="C28" s="5">
-        <v>3900</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="C29" s="5">
-        <v>4400</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="C30" s="5">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="C31" s="5">
-        <v>4700</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>431</v>
-      </c>
-      <c r="C32" s="5">
-        <v>4900</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>432</v>
-      </c>
-      <c r="C33" s="5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>433</v>
-      </c>
-      <c r="C34" s="5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="C35" s="5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="C36" s="5">
-        <v>5100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="C37" s="5">
-        <v>5600</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>437</v>
-      </c>
-      <c r="C38" s="5">
-        <v>5600</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="C39" s="5">
-        <v>5600</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="C40" s="5">
-        <v>6100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="C41" s="5">
-        <v>6200</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="C42" s="5">
-        <v>6200</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="C43" s="5">
-        <v>6200</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="C44" s="5">
-        <v>6300</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="C45" s="5">
-        <v>6500</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="C46" s="5">
-        <v>6600</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="C47" s="5">
-        <v>8800</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="C48" s="5">
-        <v>8800</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="C49" s="5">
-        <v>8800</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="C50" s="5">
-        <v>8900</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="C51" s="5">
-        <v>9300</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="C52" s="5">
-        <v>9400</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="C53" s="5">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="C54" s="5">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="C55" s="5">
-        <v>11200</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="C56" s="5">
-        <v>11200</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="C57" s="5">
-        <v>11700</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="C58" s="5">
-        <v>11700</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="C59" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="C60" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="C61" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="C62" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="C63" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="C64" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="C65" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>457</v>
-      </c>
-      <c r="C66" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="C67" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>459</v>
-      </c>
-      <c r="C68" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="C69" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="C70" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="C71" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>463</v>
-      </c>
-      <c r="C72" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="C73" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="C74" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="C75" s="5">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>467</v>
-      </c>
-      <c r="C76" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="C77" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="C78" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>470</v>
-      </c>
-      <c r="C79" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>471</v>
-      </c>
-      <c r="C80" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="C81" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="C82" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>473</v>
-      </c>
-      <c r="C83" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="C84" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="C85" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>476</v>
-      </c>
-      <c r="C86" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="C87" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="C88" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="C89" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="C90" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="C91" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="C92" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>483</v>
-      </c>
-      <c r="C93" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="C94" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="C95" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>486</v>
-      </c>
-      <c r="C96" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="C97" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="C98" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="C99" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="C100" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>491</v>
-      </c>
-      <c r="C101" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="C102" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>493</v>
-      </c>
-      <c r="C103" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>494</v>
-      </c>
-      <c r="C104" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>495</v>
-      </c>
-      <c r="C105" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="C106" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B107" s="5" t="s">
-        <v>497</v>
-      </c>
-      <c r="C107" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>498</v>
-      </c>
-      <c r="C108" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>499</v>
-      </c>
-      <c r="C109" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>500</v>
-      </c>
-      <c r="C110" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>501</v>
-      </c>
-      <c r="C111" s="5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>502</v>
-      </c>
-      <c r="C112" s="5">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>503</v>
-      </c>
-      <c r="C113" s="5">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B114" s="5" t="s">
-        <v>504</v>
-      </c>
-      <c r="C114" s="5">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>505</v>
-      </c>
-      <c r="C115" s="5">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B116" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="C116" s="5">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B117" s="5" t="s">
-        <v>507</v>
-      </c>
-      <c r="C117" s="5">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B118" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="C118" s="5">
-        <v>3100</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>509</v>
-      </c>
-      <c r="C119" s="5">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B120" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="C120" s="5">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>511</v>
-      </c>
-      <c r="C121" s="5">
-        <v>4100</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B122" s="5" t="s">
-        <v>512</v>
-      </c>
-      <c r="C122" s="5">
-        <v>4600</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>513</v>
-      </c>
-      <c r="C123" s="5">
-        <v>5100</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B124" s="5" t="s">
-        <v>514</v>
-      </c>
-      <c r="C124" s="5">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B125" s="5" t="s">
-        <v>515</v>
-      </c>
-      <c r="C125" s="5">
-        <v>5800</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B126" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="C126" s="5">
-        <v>6100</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B127" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="C127" s="5">
-        <v>6700</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B128" s="5" t="s">
-        <v>518</v>
-      </c>
-      <c r="C128" s="5">
-        <v>6700</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B129" s="5" t="s">
-        <v>519</v>
-      </c>
-      <c r="C129" s="5">
-        <v>7100</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B130" s="5" t="s">
-        <v>520</v>
-      </c>
-      <c r="C130" s="5">
-        <v>7800</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B131" s="5" t="s">
-        <v>521</v>
-      </c>
-      <c r="C131" s="5">
-        <v>7800</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B132" s="5" t="s">
-        <v>522</v>
-      </c>
-      <c r="C132" s="5">
-        <v>8600</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B133" s="5" t="s">
-        <v>523</v>
-      </c>
-      <c r="C133" s="5">
-        <v>8900</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B134" s="5" t="s">
-        <v>524</v>
-      </c>
-      <c r="C134" s="5">
-        <v>9000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19CA163-81B9-4B5D-B0E2-989B5FF2F0EE}">
-  <dimension ref="A2:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3">
-        <v>700</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>